<commit_message>
ASN+USER; YMMV; ->I TI; CLX clear TI fix; CLRMOD adapt
Fix ASN+USER return from TAM;   Fix YMMV "U" and conversion formula;   Add ->I TI message ->I to respect the sign bits; Re-enable CLX to clear TI & clear X; Swap CLRMOD sequence; Fix CLRMOD to use CLRALLMENUS;
</commit_message>
<xml_diff>
--- a/src/index spreadsheet/Conversions/YMMV/factors-2.xlsx
+++ b/src/index spreadsheet/Conversions/YMMV/factors-2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr updateLinks="always" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacomostert/Downloads/YMMV old/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacomostert/wp43s/src/index spreadsheet/Conversions/YMMV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF2B550-A06C-2F4D-BF36-0634B6D9F246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F571F1-FD12-8045-8340-3FA39ED931BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19200" xr2:uid="{928F737F-25A6-2445-BD2F-379EB36AF9BC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19160" xr2:uid="{928F737F-25A6-2445-BD2F-379EB36AF9BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -361,7 +361,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -392,6 +392,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -541,7 +547,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -616,6 +622,15 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
@@ -962,7 +977,7 @@
   <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="E37" sqref="E37:F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="82" defaultRowHeight="16"/>
@@ -1283,16 +1298,16 @@
       <c r="A37" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="26" t="s">
         <v>51</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E37" s="8">
+      <c r="E37" s="27">
         <v>1</v>
       </c>
-      <c r="F37" s="9">
+      <c r="F37" s="28">
         <f>E37*mile</f>
         <v>1.6093440000000001</v>
       </c>
@@ -1322,10 +1337,10 @@
       <c r="C38" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E38" s="8">
+      <c r="E38" s="27">
         <v>1.6</v>
       </c>
-      <c r="F38" s="9">
+      <c r="F38" s="28">
         <f>E38/mile</f>
         <v>0.99419390757973436</v>
       </c>

</xml_diff>